<commit_message>
[doc] weekly 11month 2th week
</commit_message>
<xml_diff>
--- a/doc/_meeting_weekly_doc/N2Team_WeeklySchedule_YSR.xlsx
+++ b/doc/_meeting_weekly_doc/N2Team_WeeklySchedule_YSR.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="-15" windowWidth="28020" windowHeight="3765" activeTab="1"/>
+    <workbookView xWindow="60" yWindow="-15" windowWidth="28020" windowHeight="3765"/>
   </bookViews>
   <sheets>
     <sheet name="11월3주" sheetId="2" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="53">
   <si>
     <t xml:space="preserve">작성자 </t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -166,6 +166,48 @@
   </si>
   <si>
     <t>* 주말에도 해야됨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>QuadTree의 전체적인 구조를 파악하지 못하고 있음.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">* 맵에 오브젝트 배치 및 Save,Load
+* 주인공 체력 UI, </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* QuadTree 이해와 코딩</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* QuadTree 이해와 코딩
+* 맵에 오브젝트 배치</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">오브젝트 배치 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>맵에 오브젝트 배치 및 Save</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Save, Load</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>인게임 체력 UI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전체 UI 씬 작업</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2차 발표</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -196,20 +238,32 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-* 오브젝트 Load
+* 오브젝트 배치
  - QUADTREE 
  - 충돌 데이터 산출
- - 오브젝트 srt save</t>
+</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>* QuadTree 이해와 코딩</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>오브젝트 배치 및 srt save
+    <t>오브젝트 배치 및 save, load
 바운딩 박스</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 오브젝트 배치</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11.7 ~ 11.11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 배탈이 심해서 학원에 나오지 못함.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2차 발표</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -304,7 +358,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="46">
+  <borders count="47">
     <border>
       <left/>
       <right/>
@@ -899,13 +953,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1085,6 +1152,15 @@
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1380,12 +1456,391 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22:H22"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
+  <cols>
+    <col min="1" max="1" width="12.375" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="9" style="4"/>
+    <col min="8" max="8" width="31.25" style="4" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="39" thickBot="1">
+      <c r="A1" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="14"/>
+    </row>
+    <row r="2" spans="1:8" ht="17.25" thickTop="1">
+      <c r="A2" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="16"/>
+      <c r="C2" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="18"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2" s="19"/>
+    </row>
+    <row r="3" spans="1:8" ht="56.25" customHeight="1" thickBot="1">
+      <c r="A3" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="21"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="24"/>
+    </row>
+    <row r="4" spans="1:8" ht="17.25" thickBot="1">
+      <c r="A4" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="26"/>
+      <c r="C4" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="29"/>
+    </row>
+    <row r="5" spans="1:8" ht="146.25" customHeight="1" thickTop="1">
+      <c r="A5" s="30">
+        <v>42688</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="34"/>
+    </row>
+    <row r="6" spans="1:8" ht="37.5" customHeight="1">
+      <c r="A6" s="31"/>
+      <c r="B6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="35"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="37"/>
+    </row>
+    <row r="7" spans="1:8" ht="17.25" thickBot="1">
+      <c r="A7" s="32"/>
+      <c r="B7" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="38"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="39"/>
+      <c r="H7" s="40"/>
+    </row>
+    <row r="8" spans="1:8" ht="54" customHeight="1" thickTop="1">
+      <c r="A8" s="30">
+        <v>42689</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="34"/>
+    </row>
+    <row r="9" spans="1:8" ht="66.75" customHeight="1">
+      <c r="A9" s="31"/>
+      <c r="B9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="37"/>
+    </row>
+    <row r="10" spans="1:8" ht="17.25" thickBot="1">
+      <c r="A10" s="32"/>
+      <c r="B10" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="38"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="40"/>
+    </row>
+    <row r="11" spans="1:8" ht="54" customHeight="1" thickTop="1">
+      <c r="A11" s="30">
+        <v>42690</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="34"/>
+    </row>
+    <row r="12" spans="1:8" ht="66.75" customHeight="1">
+      <c r="A12" s="31"/>
+      <c r="B12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="36"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="37"/>
+    </row>
+    <row r="13" spans="1:8" ht="44.25" customHeight="1" thickBot="1">
+      <c r="A13" s="32"/>
+      <c r="B13" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="38"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="40"/>
+    </row>
+    <row r="14" spans="1:8" ht="54" customHeight="1" thickTop="1">
+      <c r="A14" s="30">
+        <v>42691</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="33"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="34"/>
+    </row>
+    <row r="15" spans="1:8" ht="66.75" customHeight="1">
+      <c r="A15" s="31"/>
+      <c r="B15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="36"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="37"/>
+    </row>
+    <row r="16" spans="1:8" ht="53.25" customHeight="1" thickBot="1">
+      <c r="A16" s="32"/>
+      <c r="B16" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="38"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="39"/>
+      <c r="G16" s="39"/>
+      <c r="H16" s="40"/>
+    </row>
+    <row r="17" spans="1:8" ht="17.25" thickTop="1">
+      <c r="A17" s="30">
+        <v>42692</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="60" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" s="61"/>
+      <c r="E17" s="61"/>
+      <c r="F17" s="61"/>
+      <c r="G17" s="61"/>
+      <c r="H17" s="62"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="31"/>
+      <c r="B18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="43"/>
+      <c r="D18" s="44"/>
+      <c r="E18" s="44"/>
+      <c r="F18" s="44"/>
+      <c r="G18" s="44"/>
+      <c r="H18" s="45"/>
+    </row>
+    <row r="19" spans="1:8" ht="17.25" thickBot="1">
+      <c r="A19" s="32"/>
+      <c r="B19" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="36"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="36"/>
+      <c r="G19" s="36"/>
+      <c r="H19" s="37"/>
+    </row>
+    <row r="20" spans="1:8" ht="39.75" customHeight="1" thickTop="1">
+      <c r="A20" s="49" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="50"/>
+      <c r="C20" s="51"/>
+      <c r="D20" s="52"/>
+      <c r="E20" s="52"/>
+      <c r="F20" s="52"/>
+      <c r="G20" s="52"/>
+      <c r="H20" s="53"/>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="6">
+        <v>42695</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="54"/>
+      <c r="D21" s="54"/>
+      <c r="E21" s="54"/>
+      <c r="F21" s="54"/>
+      <c r="G21" s="54"/>
+      <c r="H21" s="55"/>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="6">
+        <v>42696</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="54"/>
+      <c r="D22" s="54"/>
+      <c r="E22" s="54"/>
+      <c r="F22" s="54"/>
+      <c r="G22" s="54"/>
+      <c r="H22" s="55"/>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="6">
+        <v>42697</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="54"/>
+      <c r="D23" s="54"/>
+      <c r="E23" s="54"/>
+      <c r="F23" s="54"/>
+      <c r="G23" s="54"/>
+      <c r="H23" s="55"/>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="6">
+        <v>42698</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="54"/>
+      <c r="D24" s="54"/>
+      <c r="E24" s="54"/>
+      <c r="F24" s="54"/>
+      <c r="G24" s="54"/>
+      <c r="H24" s="55"/>
+    </row>
+    <row r="25" spans="1:8" ht="17.25" customHeight="1" thickBot="1">
+      <c r="A25" s="6">
+        <v>42699</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="46"/>
+      <c r="D25" s="47"/>
+      <c r="E25" s="47"/>
+      <c r="F25" s="47"/>
+      <c r="G25" s="47"/>
+      <c r="H25" s="48"/>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="35">
+    <mergeCell ref="C25:H25"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:H20"/>
+    <mergeCell ref="C21:H21"/>
+    <mergeCell ref="C22:H22"/>
+    <mergeCell ref="C23:H23"/>
+    <mergeCell ref="C24:H24"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="C14:H14"/>
+    <mergeCell ref="C15:H15"/>
+    <mergeCell ref="C16:H16"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="C17:H17"/>
+    <mergeCell ref="C18:H18"/>
+    <mergeCell ref="C19:H19"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="C8:H8"/>
+    <mergeCell ref="C9:H9"/>
+    <mergeCell ref="C10:H10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="C11:H11"/>
+    <mergeCell ref="C12:H12"/>
+    <mergeCell ref="C13:H13"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="C6:H6"/>
+    <mergeCell ref="C7:H7"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:H3"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1399,11 +1854,11 @@
   </sheetPr>
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12:H12"/>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="12.375" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="7" width="9" style="4"/>
@@ -1437,7 +1892,7 @@
         <v>2</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="H2" s="19"/>
     </row>
@@ -1477,7 +1932,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="33" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="D5" s="33"/>
       <c r="E5" s="33"/>
@@ -1517,7 +1972,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="33" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D8" s="33"/>
       <c r="E8" s="33"/>
@@ -1530,7 +1985,9 @@
       <c r="B9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="36"/>
+      <c r="C9" s="36" t="s">
+        <v>37</v>
+      </c>
       <c r="D9" s="36"/>
       <c r="E9" s="36"/>
       <c r="F9" s="36"/>
@@ -1557,7 +2014,7 @@
         <v>8</v>
       </c>
       <c r="C11" s="33" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D11" s="33"/>
       <c r="E11" s="33"/>
@@ -1577,12 +2034,14 @@
       <c r="G12" s="36"/>
       <c r="H12" s="37"/>
     </row>
-    <row r="13" spans="1:8" ht="17.25" thickBot="1">
+    <row r="13" spans="1:8" ht="44.25" customHeight="1" thickBot="1">
       <c r="A13" s="32"/>
       <c r="B13" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="38"/>
+      <c r="C13" s="38" t="s">
+        <v>41</v>
+      </c>
       <c r="D13" s="39"/>
       <c r="E13" s="39"/>
       <c r="F13" s="39"/>
@@ -1596,7 +2055,9 @@
       <c r="B14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="33"/>
+      <c r="C14" s="33" t="s">
+        <v>49</v>
+      </c>
       <c r="D14" s="33"/>
       <c r="E14" s="33"/>
       <c r="F14" s="33"/>
@@ -1615,12 +2076,14 @@
       <c r="G15" s="36"/>
       <c r="H15" s="37"/>
     </row>
-    <row r="16" spans="1:8" ht="17.25" thickBot="1">
+    <row r="16" spans="1:8" ht="53.25" customHeight="1" thickBot="1">
       <c r="A16" s="32"/>
       <c r="B16" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="38"/>
+      <c r="C16" s="38" t="s">
+        <v>48</v>
+      </c>
       <c r="D16" s="39"/>
       <c r="E16" s="39"/>
       <c r="F16" s="39"/>
@@ -1634,7 +2097,9 @@
       <c r="B17" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="41"/>
+      <c r="C17" s="41" t="s">
+        <v>51</v>
+      </c>
       <c r="D17" s="41"/>
       <c r="E17" s="41"/>
       <c r="F17" s="41"/>
@@ -1665,13 +2130,13 @@
       <c r="G19" s="36"/>
       <c r="H19" s="37"/>
     </row>
-    <row r="20" spans="1:8" ht="32.25" customHeight="1" thickTop="1">
+    <row r="20" spans="1:8" ht="39.75" customHeight="1" thickTop="1">
       <c r="A20" s="49" t="s">
         <v>11</v>
       </c>
       <c r="B20" s="50"/>
       <c r="C20" s="51" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="D20" s="52"/>
       <c r="E20" s="52"/>
@@ -1686,7 +2151,9 @@
       <c r="B21" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="54"/>
+      <c r="C21" s="54" t="s">
+        <v>42</v>
+      </c>
       <c r="D21" s="54"/>
       <c r="E21" s="54"/>
       <c r="F21" s="54"/>
@@ -1700,7 +2167,9 @@
       <c r="B22" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="54"/>
+      <c r="C22" s="54" t="s">
+        <v>43</v>
+      </c>
       <c r="D22" s="54"/>
       <c r="E22" s="54"/>
       <c r="F22" s="54"/>
@@ -1714,7 +2183,9 @@
       <c r="B23" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="54"/>
+      <c r="C23" s="54" t="s">
+        <v>44</v>
+      </c>
       <c r="D23" s="54"/>
       <c r="E23" s="54"/>
       <c r="F23" s="54"/>
@@ -1728,7 +2199,9 @@
       <c r="B24" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="54"/>
+      <c r="C24" s="54" t="s">
+        <v>45</v>
+      </c>
       <c r="D24" s="54"/>
       <c r="E24" s="54"/>
       <c r="F24" s="54"/>
@@ -1742,7 +2215,9 @@
       <c r="B25" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="46"/>
+      <c r="C25" s="46" t="s">
+        <v>46</v>
+      </c>
       <c r="D25" s="47"/>
       <c r="E25" s="47"/>
       <c r="F25" s="47"/>
@@ -1792,7 +2267,7 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="79" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="73" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1803,11 +2278,11 @@
   </sheetPr>
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A11" sqref="A1:XFD1048576"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="12.375" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="7" width="9" style="4"/>

</xml_diff>

<commit_message>
[map_tool]  add save & static load image
</commit_message>
<xml_diff>
--- a/doc/_meeting_weekly_doc/N2Team_WeeklySchedule_YSR.xlsx
+++ b/doc/_meeting_weekly_doc/N2Team_WeeklySchedule_YSR.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="62">
   <si>
     <t xml:space="preserve">작성자 </t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -267,49 +267,53 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t xml:space="preserve">* 스카이 박스 구현 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> z버퍼의 활용을 제대로 몰랐음. (스카이 박스 랜더링은 제일 먼저 랜더링 해야되며 랜덩링 시 z버퍼를 disable 랜더링후 Enalbe로 해야됨 )
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* MFC Save
+* TileRender</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2차 발표 준비</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* MFC Save
+* TileRender</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 바닥 텍스쳐가 깨져 TileRender의 필요성을 알게됨.
+* TileRender
+  - 작업자의 마인드를 이해하게됨 
+  - 가져다 쓸 수 있지만 내가 한게 아니기에 쓰지 않음
+* MFC thApp 전역 객체을 알게됨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* MFC Save &amp; Load
+  - dlg를 통한 map 생성 구현
+  - 생성 시 image 변경 구현</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MFC Save 시 Write 함수를 통해 출력 시 문제가 있음
+save 후 타일 가로 세로 값이 ?으로 변경됨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t xml:space="preserve">* 오브잭트 배치 완료
  - 연구소
  - 드랍쉽
  - 자동차
 </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">* 스카이 박스 구현 </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> z버퍼의 활용을 제대로 몰랐음. (스카이 박스 랜더링은 제일 먼저 랜더링 해야되며 랜덩링 시 z버퍼를 disable 랜더링후 Enalbe로 해야됨 )
-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>* MFC Save
-* TileRender</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2차 발표 준비</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>* MFC Save
-* TileRender</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>* 바닥 텍스쳐가 깨져 TileRender의 필요성을 알게됨.
-* TileRender
-  - 작업자의 마인드를 이해하게됨 
-  - 가져다 쓸 수 있지만 내가 한게 아니기에 쓰지 않음
-* MFC thApp 전역 객체을 알게됨</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>* MFC Save &amp; Load
-  - dlg를 통한 map 생성 구현
-  - save
-* TileRender</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1504,8 +1508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15:H15"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -1572,7 +1576,7 @@
       <c r="G4" s="28"/>
       <c r="H4" s="29"/>
     </row>
-    <row r="5" spans="1:8" ht="146.25" customHeight="1" thickTop="1">
+    <row r="5" spans="1:8" ht="87" customHeight="1" thickTop="1">
       <c r="A5" s="30">
         <v>42688</v>
       </c>
@@ -1580,7 +1584,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="33" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="D5" s="33"/>
       <c r="E5" s="33"/>
@@ -1620,7 +1624,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D8" s="33"/>
       <c r="E8" s="33"/>
@@ -1634,7 +1638,7 @@
         <v>12</v>
       </c>
       <c r="C9" s="36" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D9" s="36"/>
       <c r="E9" s="36"/>
@@ -1662,7 +1666,7 @@
         <v>8</v>
       </c>
       <c r="C11" s="33" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D11" s="33"/>
       <c r="E11" s="33"/>
@@ -1676,7 +1680,7 @@
         <v>12</v>
       </c>
       <c r="C12" s="36" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D12" s="36"/>
       <c r="E12" s="36"/>
@@ -1690,7 +1694,7 @@
         <v>20</v>
       </c>
       <c r="C13" s="38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D13" s="39"/>
       <c r="E13" s="39"/>
@@ -1706,7 +1710,7 @@
         <v>9</v>
       </c>
       <c r="C14" s="33" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D14" s="33"/>
       <c r="E14" s="33"/>
@@ -1719,7 +1723,9 @@
       <c r="B15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="36"/>
+      <c r="C15" s="36" t="s">
+        <v>60</v>
+      </c>
       <c r="D15" s="36"/>
       <c r="E15" s="36"/>
       <c r="F15" s="36"/>
@@ -1732,7 +1738,7 @@
         <v>20</v>
       </c>
       <c r="C16" s="38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D16" s="39"/>
       <c r="E16" s="39"/>

</xml_diff>

<commit_message>
[map&doc] add solution filter&Weekly doc
</commit_message>
<xml_diff>
--- a/doc/_meeting_weekly_doc/N2Team_WeeklySchedule_YSR.xlsx
+++ b/doc/_meeting_weekly_doc/N2Team_WeeklySchedule_YSR.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="69">
   <si>
     <t xml:space="preserve">작성자 </t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -170,11 +170,6 @@
   </si>
   <si>
     <t>QuadTree의 전체적인 구조를 파악하지 못하고 있음.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">* 맵에 오브젝트 배치 및 Save,Load
-* 주인공 체력 UI, </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -263,10 +258,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2차 발표</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">* 스카이 박스 구현 </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -304,16 +295,57 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>MFC Save 시 Write 함수를 통해 출력 시 문제가 있음
-save 후 타일 가로 세로 값이 ?으로 변경됨</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">* 오브잭트 배치 완료
  - 연구소
  - 드랍쉽
  - 자동차
 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MFC Load</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* MFC Load &amp; Map 퀄리티</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MFC Load &amp; 지형 높이 컨트롤</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지형 높이 컨트롤</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">MFC Save 시 Write 함수를 통해 출력 시 문제가 있음
+save 후 타일 가로 세로 값이 ?으로 변경됨
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>변수 값 출력 후 값이? 됨 따라서 일회성 변수를 만들어 넘긴후 일회성 변수를 출력</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>맵 퀄리티 높이기(tile render)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 2차 발표
+* MFC Save 구현
+ - 세이브 버그 fix</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">* 맵에 오브젝트 배치 및 Save,Load
+* 주인공 체력 UI, </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">* 맵에 오브젝트 배치 및 Save,Load
+* 주인공 체력 UI, </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -408,7 +440,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="47">
+  <borders count="50">
     <border>
       <left/>
       <right/>
@@ -1016,13 +1048,44 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1059,6 +1122,108 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1098,100 +1263,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1506,10 +1578,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -1521,282 +1596,288 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="39" thickBot="1">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="14"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="48"/>
     </row>
     <row r="2" spans="1:8" ht="17.25" thickTop="1">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="17" t="s">
+      <c r="B2" s="50"/>
+      <c r="C2" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="18"/>
-      <c r="E2" s="16"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="50"/>
       <c r="F2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="H2" s="19"/>
+      <c r="G2" s="51" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" s="53"/>
     </row>
     <row r="3" spans="1:8" ht="56.25" customHeight="1" thickBot="1">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="24"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="56" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="58"/>
     </row>
     <row r="4" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="27" t="s">
+      <c r="B4" s="41"/>
+      <c r="C4" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="29"/>
-    </row>
-    <row r="5" spans="1:8" ht="87" customHeight="1" thickTop="1">
-      <c r="A5" s="30">
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="44"/>
+    </row>
+    <row r="5" spans="1:8" ht="74.25" customHeight="1" thickTop="1">
+      <c r="A5" s="22">
         <v>42688</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="33" t="s">
-        <v>61</v>
-      </c>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="34"/>
-    </row>
-    <row r="6" spans="1:8" ht="37.5" customHeight="1">
-      <c r="A6" s="31"/>
+      <c r="C5" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="26"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="23"/>
       <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="35"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
-      <c r="G6" s="36"/>
-      <c r="H6" s="37"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="28"/>
     </row>
     <row r="7" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A7" s="32"/>
+      <c r="A7" s="24"/>
       <c r="B7" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="38"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="40"/>
-    </row>
-    <row r="8" spans="1:8" ht="54" customHeight="1" thickTop="1">
-      <c r="A8" s="30">
+      <c r="C7" s="29"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="31"/>
+    </row>
+    <row r="8" spans="1:8" ht="24" customHeight="1" thickTop="1">
+      <c r="A8" s="22">
         <v>42689</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="34"/>
-    </row>
-    <row r="9" spans="1:8" ht="66.75" customHeight="1">
-      <c r="A9" s="31"/>
+      <c r="C8" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="26"/>
+    </row>
+    <row r="9" spans="1:8" ht="40.5" customHeight="1">
+      <c r="A9" s="23"/>
       <c r="B9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="37"/>
+      <c r="C9" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="28"/>
     </row>
     <row r="10" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A10" s="32"/>
+      <c r="A10" s="24"/>
       <c r="B10" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="38"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="40"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="31"/>
     </row>
     <row r="11" spans="1:8" ht="54" customHeight="1" thickTop="1">
-      <c r="A11" s="30">
+      <c r="A11" s="22">
         <v>42690</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="33" t="s">
-        <v>57</v>
-      </c>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="34"/>
+      <c r="C11" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="26"/>
     </row>
     <row r="12" spans="1:8" ht="126" customHeight="1">
-      <c r="A12" s="31"/>
+      <c r="A12" s="23"/>
       <c r="B12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="36" t="s">
-        <v>58</v>
-      </c>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="37"/>
+      <c r="C12" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="28"/>
     </row>
     <row r="13" spans="1:8" ht="44.25" customHeight="1" thickBot="1">
-      <c r="A13" s="32"/>
+      <c r="A13" s="24"/>
       <c r="B13" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="39"/>
-      <c r="H13" s="40"/>
-    </row>
-    <row r="14" spans="1:8" ht="91.5" customHeight="1" thickTop="1">
-      <c r="A14" s="30">
+      <c r="C13" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="31"/>
+    </row>
+    <row r="14" spans="1:8" ht="66" customHeight="1" thickTop="1">
+      <c r="A14" s="22">
         <v>42691</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="33" t="s">
-        <v>59</v>
-      </c>
-      <c r="D14" s="33"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="34"/>
-    </row>
-    <row r="15" spans="1:8" ht="66.75" customHeight="1">
-      <c r="A15" s="31"/>
+      <c r="C14" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="26"/>
+    </row>
+    <row r="15" spans="1:8" ht="45.75" customHeight="1">
+      <c r="A15" s="23"/>
       <c r="B15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="36" t="s">
-        <v>60</v>
-      </c>
-      <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="37"/>
-    </row>
-    <row r="16" spans="1:8" ht="53.25" customHeight="1" thickBot="1">
-      <c r="A16" s="32"/>
+      <c r="C15" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="28"/>
+    </row>
+    <row r="16" spans="1:8" ht="27.75" customHeight="1" thickBot="1">
+      <c r="A16" s="24"/>
       <c r="B16" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="38" t="s">
-        <v>56</v>
-      </c>
-      <c r="D16" s="39"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="39"/>
-      <c r="G16" s="39"/>
-      <c r="H16" s="40"/>
-    </row>
-    <row r="17" spans="1:8" ht="17.25" thickTop="1">
-      <c r="A17" s="30">
+      <c r="C16" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="31"/>
+    </row>
+    <row r="17" spans="1:8" ht="64.5" customHeight="1" thickTop="1">
+      <c r="A17" s="22">
         <v>42692</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="41" t="s">
-        <v>52</v>
-      </c>
-      <c r="D17" s="42"/>
-      <c r="E17" s="42"/>
-      <c r="F17" s="42"/>
-      <c r="G17" s="42"/>
-      <c r="H17" s="43"/>
+      <c r="C17" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17" s="33"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="33"/>
+      <c r="G17" s="33"/>
+      <c r="H17" s="34"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="31"/>
+      <c r="A18" s="23"/>
       <c r="B18" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="44"/>
-      <c r="D18" s="45"/>
-      <c r="E18" s="45"/>
-      <c r="F18" s="45"/>
-      <c r="G18" s="45"/>
-      <c r="H18" s="46"/>
+      <c r="C18" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="37"/>
     </row>
     <row r="19" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A19" s="32"/>
-      <c r="B19" s="3" t="s">
+      <c r="A19" s="23"/>
+      <c r="B19" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="36"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="36"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="36"/>
-      <c r="H19" s="37"/>
-    </row>
-    <row r="20" spans="1:8" ht="39.75" customHeight="1" thickTop="1">
-      <c r="A20" s="50" t="s">
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="39"/>
+    </row>
+    <row r="20" spans="1:8" ht="39.75" customHeight="1">
+      <c r="A20" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="51"/>
-      <c r="C20" s="52"/>
-      <c r="D20" s="53"/>
-      <c r="E20" s="53"/>
-      <c r="F20" s="53"/>
-      <c r="G20" s="53"/>
-      <c r="H20" s="54"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="19"/>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="6">
@@ -1805,12 +1886,14 @@
       <c r="B21" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="55"/>
-      <c r="D21" s="55"/>
-      <c r="E21" s="55"/>
-      <c r="F21" s="55"/>
-      <c r="G21" s="55"/>
-      <c r="H21" s="56"/>
+      <c r="C21" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="21"/>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="6">
@@ -1819,12 +1902,14 @@
       <c r="B22" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="55"/>
-      <c r="D22" s="55"/>
-      <c r="E22" s="55"/>
-      <c r="F22" s="55"/>
-      <c r="G22" s="55"/>
-      <c r="H22" s="56"/>
+      <c r="C22" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="21"/>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="6">
@@ -1833,12 +1918,14 @@
       <c r="B23" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="55"/>
-      <c r="D23" s="55"/>
-      <c r="E23" s="55"/>
-      <c r="F23" s="55"/>
-      <c r="G23" s="55"/>
-      <c r="H23" s="56"/>
+      <c r="C23" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="21"/>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="6">
@@ -1847,39 +1934,56 @@
       <c r="B24" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="55"/>
-      <c r="D24" s="55"/>
-      <c r="E24" s="55"/>
-      <c r="F24" s="55"/>
-      <c r="G24" s="55"/>
-      <c r="H24" s="56"/>
+      <c r="C24" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="21"/>
     </row>
     <row r="25" spans="1:8" ht="17.25" customHeight="1" thickBot="1">
-      <c r="A25" s="6">
+      <c r="A25" s="8">
         <v>42699</v>
       </c>
       <c r="B25" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="47"/>
-      <c r="D25" s="48"/>
-      <c r="E25" s="48"/>
-      <c r="F25" s="48"/>
-      <c r="G25" s="48"/>
-      <c r="H25" s="49"/>
+      <c r="C25" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="14"/>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="C25:H25"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:H20"/>
-    <mergeCell ref="C21:H21"/>
-    <mergeCell ref="C22:H22"/>
-    <mergeCell ref="C23:H23"/>
-    <mergeCell ref="C24:H24"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="C6:H6"/>
+    <mergeCell ref="C7:H7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="C8:H8"/>
+    <mergeCell ref="C9:H9"/>
+    <mergeCell ref="C10:H10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="C11:H11"/>
+    <mergeCell ref="C12:H12"/>
+    <mergeCell ref="C13:H13"/>
     <mergeCell ref="A14:A16"/>
     <mergeCell ref="C14:H14"/>
     <mergeCell ref="C15:H15"/>
@@ -1888,30 +1992,17 @@
     <mergeCell ref="C17:H17"/>
     <mergeCell ref="C18:H18"/>
     <mergeCell ref="C19:H19"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="C8:H8"/>
-    <mergeCell ref="C9:H9"/>
-    <mergeCell ref="C10:H10"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="C11:H11"/>
-    <mergeCell ref="C12:H12"/>
-    <mergeCell ref="C13:H13"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:H4"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="C5:H5"/>
-    <mergeCell ref="C6:H6"/>
-    <mergeCell ref="C7:H7"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="C25:H25"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:H20"/>
+    <mergeCell ref="C21:H21"/>
+    <mergeCell ref="C22:H22"/>
+    <mergeCell ref="C23:H23"/>
+    <mergeCell ref="C24:H24"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1923,7 +2014,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -1935,282 +2026,282 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="39" thickBot="1">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="14"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="48"/>
     </row>
     <row r="2" spans="1:8" ht="17.25" thickTop="1">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="17" t="s">
+      <c r="B2" s="50"/>
+      <c r="C2" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="18"/>
-      <c r="E2" s="16"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="50"/>
       <c r="F2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="H2" s="19"/>
+      <c r="G2" s="51" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" s="53"/>
     </row>
     <row r="3" spans="1:8" ht="56.25" customHeight="1" thickBot="1">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="22" t="s">
+      <c r="B3" s="55"/>
+      <c r="C3" s="56" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="24"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="58"/>
     </row>
     <row r="4" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="27" t="s">
+      <c r="B4" s="41"/>
+      <c r="C4" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="29"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="44"/>
     </row>
     <row r="5" spans="1:8" ht="146.25" customHeight="1" thickTop="1">
-      <c r="A5" s="30">
+      <c r="A5" s="22">
         <v>42681</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="33" t="s">
-        <v>47</v>
-      </c>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="34"/>
+      <c r="C5" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="26"/>
     </row>
     <row r="6" spans="1:8" ht="37.5" customHeight="1">
-      <c r="A6" s="31"/>
+      <c r="A6" s="23"/>
       <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="35"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
-      <c r="G6" s="36"/>
-      <c r="H6" s="37"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="28"/>
     </row>
     <row r="7" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A7" s="32"/>
+      <c r="A7" s="24"/>
       <c r="B7" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="38"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="40"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="31"/>
     </row>
     <row r="8" spans="1:8" ht="54" customHeight="1" thickTop="1">
-      <c r="A8" s="30">
+      <c r="A8" s="22">
         <v>42682</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="34"/>
+      <c r="C8" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="26"/>
     </row>
     <row r="9" spans="1:8" ht="66.75" customHeight="1">
-      <c r="A9" s="31"/>
+      <c r="A9" s="23"/>
       <c r="B9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="36" t="s">
+      <c r="C9" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="37"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="28"/>
     </row>
     <row r="10" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A10" s="32"/>
+      <c r="A10" s="24"/>
       <c r="B10" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="38"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="40"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="31"/>
     </row>
     <row r="11" spans="1:8" ht="54" customHeight="1" thickTop="1">
-      <c r="A11" s="30">
+      <c r="A11" s="22">
         <v>42683</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="34"/>
+      <c r="C11" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="26"/>
     </row>
     <row r="12" spans="1:8" ht="66.75" customHeight="1">
-      <c r="A12" s="31"/>
+      <c r="A12" s="23"/>
       <c r="B12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="37"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="28"/>
     </row>
     <row r="13" spans="1:8" ht="44.25" customHeight="1" thickBot="1">
-      <c r="A13" s="32"/>
+      <c r="A13" s="24"/>
       <c r="B13" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="38" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="39"/>
-      <c r="H13" s="40"/>
+      <c r="C13" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="31"/>
     </row>
     <row r="14" spans="1:8" ht="54" customHeight="1" thickTop="1">
-      <c r="A14" s="30">
+      <c r="A14" s="22">
         <v>42684</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="33" t="s">
-        <v>49</v>
-      </c>
-      <c r="D14" s="33"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="34"/>
+      <c r="C14" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="26"/>
     </row>
     <row r="15" spans="1:8" ht="66.75" customHeight="1">
-      <c r="A15" s="31"/>
+      <c r="A15" s="23"/>
       <c r="B15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="36"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="37"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="28"/>
     </row>
     <row r="16" spans="1:8" ht="53.25" customHeight="1" thickBot="1">
-      <c r="A16" s="32"/>
+      <c r="A16" s="24"/>
       <c r="B16" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="D16" s="39"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="39"/>
-      <c r="G16" s="39"/>
-      <c r="H16" s="40"/>
+      <c r="C16" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="31"/>
     </row>
     <row r="17" spans="1:8" ht="18" thickTop="1">
-      <c r="A17" s="30">
+      <c r="A17" s="22">
         <v>42685</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="57" t="s">
-        <v>51</v>
-      </c>
-      <c r="D17" s="57"/>
-      <c r="E17" s="57"/>
-      <c r="F17" s="57"/>
-      <c r="G17" s="57"/>
-      <c r="H17" s="58"/>
+      <c r="C17" s="60" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="60"/>
+      <c r="E17" s="60"/>
+      <c r="F17" s="60"/>
+      <c r="G17" s="60"/>
+      <c r="H17" s="61"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="31"/>
+      <c r="A18" s="23"/>
       <c r="B18" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="44"/>
-      <c r="D18" s="45"/>
-      <c r="E18" s="45"/>
-      <c r="F18" s="45"/>
-      <c r="G18" s="45"/>
-      <c r="H18" s="46"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="37"/>
     </row>
     <row r="19" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A19" s="32"/>
+      <c r="A19" s="24"/>
       <c r="B19" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="36"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="36"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="36"/>
-      <c r="H19" s="37"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="28"/>
     </row>
     <row r="20" spans="1:8" ht="39.75" customHeight="1" thickTop="1">
-      <c r="A20" s="50" t="s">
+      <c r="A20" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="51"/>
-      <c r="C20" s="52" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20" s="53"/>
-      <c r="E20" s="53"/>
-      <c r="F20" s="53"/>
-      <c r="G20" s="53"/>
-      <c r="H20" s="54"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="19"/>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="6">
@@ -2219,14 +2310,14 @@
       <c r="B21" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="55" t="s">
-        <v>42</v>
-      </c>
-      <c r="D21" s="55"/>
-      <c r="E21" s="55"/>
-      <c r="F21" s="55"/>
-      <c r="G21" s="55"/>
-      <c r="H21" s="56"/>
+      <c r="C21" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="21"/>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="6">
@@ -2235,14 +2326,14 @@
       <c r="B22" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="55" t="s">
-        <v>43</v>
-      </c>
-      <c r="D22" s="55"/>
-      <c r="E22" s="55"/>
-      <c r="F22" s="55"/>
-      <c r="G22" s="55"/>
-      <c r="H22" s="56"/>
+      <c r="C22" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="21"/>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="6">
@@ -2251,14 +2342,14 @@
       <c r="B23" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="55" t="s">
-        <v>44</v>
-      </c>
-      <c r="D23" s="55"/>
-      <c r="E23" s="55"/>
-      <c r="F23" s="55"/>
-      <c r="G23" s="55"/>
-      <c r="H23" s="56"/>
+      <c r="C23" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="21"/>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="6">
@@ -2267,14 +2358,14 @@
       <c r="B24" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="55" t="s">
-        <v>45</v>
-      </c>
-      <c r="D24" s="55"/>
-      <c r="E24" s="55"/>
-      <c r="F24" s="55"/>
-      <c r="G24" s="55"/>
-      <c r="H24" s="56"/>
+      <c r="C24" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="21"/>
     </row>
     <row r="25" spans="1:8" ht="17.25" customHeight="1" thickBot="1">
       <c r="A25" s="6">
@@ -2283,27 +2374,40 @@
       <c r="B25" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="47" t="s">
-        <v>46</v>
-      </c>
-      <c r="D25" s="48"/>
-      <c r="E25" s="48"/>
-      <c r="F25" s="48"/>
-      <c r="G25" s="48"/>
-      <c r="H25" s="49"/>
+      <c r="C25" s="59" t="s">
+        <v>45</v>
+      </c>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="14"/>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="C25:H25"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:H20"/>
-    <mergeCell ref="C21:H21"/>
-    <mergeCell ref="C22:H22"/>
-    <mergeCell ref="C23:H23"/>
-    <mergeCell ref="C24:H24"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="C6:H6"/>
+    <mergeCell ref="C7:H7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="C8:H8"/>
+    <mergeCell ref="C9:H9"/>
+    <mergeCell ref="C10:H10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="C11:H11"/>
+    <mergeCell ref="C12:H12"/>
+    <mergeCell ref="C13:H13"/>
     <mergeCell ref="A14:A16"/>
     <mergeCell ref="C14:H14"/>
     <mergeCell ref="C15:H15"/>
@@ -2312,26 +2416,13 @@
     <mergeCell ref="C17:H17"/>
     <mergeCell ref="C18:H18"/>
     <mergeCell ref="C19:H19"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="C8:H8"/>
-    <mergeCell ref="C9:H9"/>
-    <mergeCell ref="C10:H10"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="C11:H11"/>
-    <mergeCell ref="C12:H12"/>
-    <mergeCell ref="C13:H13"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:H4"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="C5:H5"/>
-    <mergeCell ref="C6:H6"/>
-    <mergeCell ref="C7:H7"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="C25:H25"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:H20"/>
+    <mergeCell ref="C21:H21"/>
+    <mergeCell ref="C22:H22"/>
+    <mergeCell ref="C23:H23"/>
+    <mergeCell ref="C24:H24"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -2359,294 +2450,294 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="39" thickBot="1">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="14"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="48"/>
     </row>
     <row r="2" spans="1:8" ht="17.25" thickTop="1">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="17" t="s">
+      <c r="B2" s="50"/>
+      <c r="C2" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="18"/>
-      <c r="E2" s="16"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="50"/>
       <c r="F2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="17" t="s">
+      <c r="G2" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="19"/>
+      <c r="H2" s="53"/>
     </row>
     <row r="3" spans="1:8" ht="56.25" customHeight="1" thickBot="1">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="22" t="s">
+      <c r="B3" s="55"/>
+      <c r="C3" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="24"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="58"/>
     </row>
     <row r="4" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="27" t="s">
+      <c r="B4" s="41"/>
+      <c r="C4" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="29"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="44"/>
     </row>
     <row r="5" spans="1:8" ht="45" customHeight="1" thickTop="1">
-      <c r="A5" s="30">
+      <c r="A5" s="22">
         <v>42674</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="33" t="s">
+      <c r="C5" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="34"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="26"/>
     </row>
     <row r="6" spans="1:8" ht="37.5" customHeight="1">
-      <c r="A6" s="31"/>
+      <c r="A6" s="23"/>
       <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="35" t="s">
+      <c r="C6" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="36"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
-      <c r="G6" s="36"/>
-      <c r="H6" s="37"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="28"/>
     </row>
     <row r="7" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A7" s="32"/>
+      <c r="A7" s="24"/>
       <c r="B7" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="38" t="s">
+      <c r="C7" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="40"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="31"/>
     </row>
     <row r="8" spans="1:8" ht="54" customHeight="1" thickTop="1">
-      <c r="A8" s="59">
+      <c r="A8" s="62">
         <v>42675</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="33" t="s">
+      <c r="C8" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="34"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="26"/>
     </row>
     <row r="9" spans="1:8" ht="66.75" customHeight="1">
-      <c r="A9" s="60"/>
+      <c r="A9" s="63"/>
       <c r="B9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="36" t="s">
+      <c r="C9" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="37"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="28"/>
     </row>
     <row r="10" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A10" s="61"/>
+      <c r="A10" s="64"/>
       <c r="B10" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="38" t="s">
+      <c r="C10" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="40"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="31"/>
     </row>
     <row r="11" spans="1:8" ht="54" customHeight="1" thickTop="1">
-      <c r="A11" s="59">
+      <c r="A11" s="62">
         <v>42676</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="33" t="s">
+      <c r="C11" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="34"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="26"/>
     </row>
     <row r="12" spans="1:8" ht="66.75" customHeight="1">
-      <c r="A12" s="60"/>
+      <c r="A12" s="63"/>
       <c r="B12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="36" t="s">
+      <c r="C12" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="37"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="28"/>
     </row>
     <row r="13" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A13" s="61"/>
+      <c r="A13" s="64"/>
       <c r="B13" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="38" t="s">
+      <c r="C13" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="39"/>
-      <c r="H13" s="40"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="31"/>
     </row>
     <row r="14" spans="1:8" ht="54" customHeight="1" thickTop="1">
-      <c r="A14" s="59">
+      <c r="A14" s="62">
         <v>42677</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="33" t="s">
+      <c r="C14" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="33"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="34"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="26"/>
     </row>
     <row r="15" spans="1:8" ht="66.75" customHeight="1">
-      <c r="A15" s="60"/>
+      <c r="A15" s="63"/>
       <c r="B15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="36" t="s">
+      <c r="C15" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="37"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="28"/>
     </row>
     <row r="16" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A16" s="61"/>
+      <c r="A16" s="64"/>
       <c r="B16" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="38" t="s">
+      <c r="C16" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="39"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="39"/>
-      <c r="G16" s="39"/>
-      <c r="H16" s="40"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="31"/>
     </row>
     <row r="17" spans="1:8" ht="18" thickTop="1">
-      <c r="A17" s="31">
+      <c r="A17" s="23">
         <v>42678</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="57" t="s">
+      <c r="C17" s="60" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="57"/>
-      <c r="E17" s="57"/>
-      <c r="F17" s="57"/>
-      <c r="G17" s="57"/>
-      <c r="H17" s="58"/>
+      <c r="D17" s="60"/>
+      <c r="E17" s="60"/>
+      <c r="F17" s="60"/>
+      <c r="G17" s="60"/>
+      <c r="H17" s="61"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="31"/>
+      <c r="A18" s="23"/>
       <c r="B18" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="44"/>
-      <c r="D18" s="45"/>
-      <c r="E18" s="45"/>
-      <c r="F18" s="45"/>
-      <c r="G18" s="45"/>
-      <c r="H18" s="46"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="37"/>
     </row>
     <row r="19" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A19" s="62"/>
+      <c r="A19" s="65"/>
       <c r="B19" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="36" t="s">
+      <c r="C19" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="D19" s="36"/>
-      <c r="E19" s="36"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="36"/>
-      <c r="H19" s="37"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="28"/>
     </row>
     <row r="20" spans="1:8" ht="32.25" customHeight="1">
-      <c r="A20" s="50" t="s">
+      <c r="A20" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="51"/>
-      <c r="C20" s="52" t="s">
+      <c r="B20" s="16"/>
+      <c r="C20" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="D20" s="53"/>
-      <c r="E20" s="53"/>
-      <c r="F20" s="53"/>
-      <c r="G20" s="53"/>
-      <c r="H20" s="54"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="19"/>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="6">
@@ -2655,14 +2746,14 @@
       <c r="B21" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="55" t="s">
+      <c r="C21" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="D21" s="55"/>
-      <c r="E21" s="55"/>
-      <c r="F21" s="55"/>
-      <c r="G21" s="55"/>
-      <c r="H21" s="56"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="21"/>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="6">
@@ -2671,14 +2762,14 @@
       <c r="B22" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="55" t="s">
+      <c r="C22" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="D22" s="55"/>
-      <c r="E22" s="55"/>
-      <c r="F22" s="55"/>
-      <c r="G22" s="55"/>
-      <c r="H22" s="56"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="21"/>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="6">
@@ -2687,14 +2778,14 @@
       <c r="B23" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="55" t="s">
+      <c r="C23" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="D23" s="55"/>
-      <c r="E23" s="55"/>
-      <c r="F23" s="55"/>
-      <c r="G23" s="55"/>
-      <c r="H23" s="56"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="21"/>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="6">
@@ -2703,14 +2794,14 @@
       <c r="B24" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="55" t="s">
+      <c r="C24" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="D24" s="55"/>
-      <c r="E24" s="55"/>
-      <c r="F24" s="55"/>
-      <c r="G24" s="55"/>
-      <c r="H24" s="56"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="21"/>
     </row>
     <row r="25" spans="1:8" ht="17.25" customHeight="1" thickBot="1">
       <c r="A25" s="8">
@@ -2719,26 +2810,33 @@
       <c r="B25" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="47" t="s">
+      <c r="C25" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="D25" s="48"/>
-      <c r="E25" s="48"/>
-      <c r="F25" s="48"/>
-      <c r="G25" s="48"/>
-      <c r="H25" s="49"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="14"/>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="C9:H9"/>
-    <mergeCell ref="C12:H12"/>
-    <mergeCell ref="C15:H15"/>
-    <mergeCell ref="C20:H20"/>
-    <mergeCell ref="C19:H19"/>
-    <mergeCell ref="C18:H18"/>
+    <mergeCell ref="C21:H21"/>
+    <mergeCell ref="C22:H22"/>
+    <mergeCell ref="C23:H23"/>
+    <mergeCell ref="C24:H24"/>
+    <mergeCell ref="C25:H25"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:E2"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="A5:A7"/>
@@ -2755,19 +2853,12 @@
     <mergeCell ref="C16:H16"/>
     <mergeCell ref="C17:H17"/>
     <mergeCell ref="C6:H6"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C3:H3"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="C4:H4"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="C21:H21"/>
-    <mergeCell ref="C22:H22"/>
-    <mergeCell ref="C23:H23"/>
-    <mergeCell ref="C24:H24"/>
-    <mergeCell ref="C25:H25"/>
+    <mergeCell ref="C9:H9"/>
+    <mergeCell ref="C12:H12"/>
+    <mergeCell ref="C15:H15"/>
+    <mergeCell ref="C20:H20"/>
+    <mergeCell ref="C19:H19"/>
+    <mergeCell ref="C18:H18"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[map] frustum culling sample
</commit_message>
<xml_diff>
--- a/doc/_meeting_weekly_doc/N2Team_WeeklySchedule_YSR.xlsx
+++ b/doc/_meeting_weekly_doc/N2Team_WeeklySchedule_YSR.xlsx
@@ -7,16 +7,17 @@
     <workbookView xWindow="60" yWindow="-15" windowWidth="28020" windowHeight="3765"/>
   </bookViews>
   <sheets>
-    <sheet name="11월3주" sheetId="2" r:id="rId1"/>
-    <sheet name="11월 2주" sheetId="3" r:id="rId2"/>
-    <sheet name="11월1주" sheetId="1" r:id="rId3"/>
+    <sheet name="11월4주" sheetId="4" r:id="rId1"/>
+    <sheet name="11월3주" sheetId="2" r:id="rId2"/>
+    <sheet name="11월 2주" sheetId="3" r:id="rId3"/>
+    <sheet name="11월1주" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="75">
   <si>
     <t xml:space="preserve">작성자 </t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -346,6 +347,34 @@
   <si>
     <t xml:space="preserve">* 맵에 오브젝트 배치 및 Save,Load
 * 주인공 체력 UI, </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* TileRender</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 프로스텀 과 쿼드 트리의 상관관계를 이해하지 못함.
+* TileRender는 끝내지 못하고 바로 위 상관관계에 대한 공부 및 프로스텀 코드 작성
+* 점심에 팀회식겸 점심에 술한잔에 머리가 어지러워 점심 이후로 집중을 잘 하지 못함
+  - 이제 술은 점심에 안마실거라고 다짐</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 2차 발표 후 늘어짐.  내일부터 열심히 해야지…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* TileRender</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* TileRender
+* Frustum 코드 작성 및 이해</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* Frustum 구현</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1125,6 +1154,117 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1152,124 +1292,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1578,13 +1607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21:H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -1596,288 +1622,280 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="39" thickBot="1">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="48"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="15"/>
     </row>
     <row r="2" spans="1:8" ht="17.25" thickTop="1">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="51" t="s">
+      <c r="B2" s="17"/>
+      <c r="C2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="52"/>
-      <c r="E2" s="50"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="17"/>
       <c r="F2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="51" t="s">
+      <c r="G2" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="H2" s="53"/>
+      <c r="H2" s="20"/>
     </row>
     <row r="3" spans="1:8" ht="56.25" customHeight="1" thickBot="1">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="56" t="s">
-        <v>68</v>
-      </c>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="58"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="25"/>
     </row>
     <row r="4" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="41"/>
-      <c r="C4" s="42" t="s">
+      <c r="B4" s="27"/>
+      <c r="C4" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="44"/>
-    </row>
-    <row r="5" spans="1:8" ht="74.25" customHeight="1" thickTop="1">
-      <c r="A5" s="22">
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="30"/>
+    </row>
+    <row r="5" spans="1:8" ht="34.5" customHeight="1" thickTop="1">
+      <c r="A5" s="31">
         <v>42688</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="26"/>
+      <c r="C5" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="35"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="23"/>
+      <c r="A6" s="32"/>
       <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="45"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="28"/>
+      <c r="C6" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="38"/>
     </row>
     <row r="7" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A7" s="24"/>
+      <c r="A7" s="33"/>
       <c r="B7" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="29"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="31"/>
-    </row>
-    <row r="8" spans="1:8" ht="24" customHeight="1" thickTop="1">
-      <c r="A8" s="22">
+      <c r="C7" s="39" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="41"/>
+    </row>
+    <row r="8" spans="1:8" ht="63.75" customHeight="1" thickTop="1">
+      <c r="A8" s="31">
         <v>42689</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="26"/>
-    </row>
-    <row r="9" spans="1:8" ht="40.5" customHeight="1">
-      <c r="A9" s="23"/>
+      <c r="C8" s="34" t="s">
+        <v>73</v>
+      </c>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="35"/>
+    </row>
+    <row r="9" spans="1:8" ht="76.5" customHeight="1">
+      <c r="A9" s="32"/>
       <c r="B9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="28"/>
-    </row>
-    <row r="10" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A10" s="24"/>
+      <c r="C9" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="38"/>
+    </row>
+    <row r="10" spans="1:8" ht="24" customHeight="1" thickBot="1">
+      <c r="A10" s="33"/>
       <c r="B10" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="29"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="31"/>
+      <c r="C10" s="39" t="s">
+        <v>74</v>
+      </c>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="41"/>
     </row>
     <row r="11" spans="1:8" ht="54" customHeight="1" thickTop="1">
-      <c r="A11" s="22">
+      <c r="A11" s="31">
         <v>42690</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="26"/>
-    </row>
-    <row r="12" spans="1:8" ht="126" customHeight="1">
-      <c r="A12" s="23"/>
+      <c r="C11" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="35"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="32"/>
       <c r="B12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="28"/>
-    </row>
-    <row r="13" spans="1:8" ht="44.25" customHeight="1" thickBot="1">
-      <c r="A13" s="24"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="38"/>
+    </row>
+    <row r="13" spans="1:8" ht="17.25" thickBot="1">
+      <c r="A13" s="33"/>
       <c r="B13" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="D13" s="30"/>
-      <c r="E13" s="30"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="30"/>
-      <c r="H13" s="31"/>
-    </row>
-    <row r="14" spans="1:8" ht="66" customHeight="1" thickTop="1">
-      <c r="A14" s="22">
+      <c r="C13" s="39"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="41"/>
+    </row>
+    <row r="14" spans="1:8" ht="18" thickTop="1">
+      <c r="A14" s="31">
         <v>42691</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="26"/>
-    </row>
-    <row r="15" spans="1:8" ht="45.75" customHeight="1">
-      <c r="A15" s="23"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="35"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="32"/>
       <c r="B15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="27" t="s">
-        <v>63</v>
-      </c>
-      <c r="D15" s="27"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="28"/>
-    </row>
-    <row r="16" spans="1:8" ht="27.75" customHeight="1" thickBot="1">
-      <c r="A16" s="24"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="38"/>
+    </row>
+    <row r="16" spans="1:8" ht="17.25" thickBot="1">
+      <c r="A16" s="33"/>
       <c r="B16" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="31"/>
-    </row>
-    <row r="17" spans="1:8" ht="64.5" customHeight="1" thickTop="1">
-      <c r="A17" s="22">
+      <c r="C16" s="39"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="40"/>
+      <c r="H16" s="41"/>
+    </row>
+    <row r="17" spans="1:8" ht="18" thickTop="1">
+      <c r="A17" s="31">
         <v>42692</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="D17" s="33"/>
-      <c r="E17" s="33"/>
-      <c r="F17" s="33"/>
-      <c r="G17" s="33"/>
-      <c r="H17" s="34"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="43"/>
+      <c r="H17" s="44"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="23"/>
+      <c r="A18" s="32"/>
       <c r="B18" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="37"/>
+      <c r="C18" s="45"/>
+      <c r="D18" s="46"/>
+      <c r="E18" s="46"/>
+      <c r="F18" s="46"/>
+      <c r="G18" s="46"/>
+      <c r="H18" s="47"/>
     </row>
     <row r="19" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A19" s="23"/>
+      <c r="A19" s="32"/>
       <c r="B19" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="38"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="38"/>
-      <c r="G19" s="38"/>
-      <c r="H19" s="39"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="48"/>
+      <c r="E19" s="48"/>
+      <c r="F19" s="48"/>
+      <c r="G19" s="48"/>
+      <c r="H19" s="49"/>
     </row>
     <row r="20" spans="1:8" ht="39.75" customHeight="1">
-      <c r="A20" s="15" t="s">
+      <c r="A20" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="16"/>
-      <c r="C20" s="17" t="s">
+      <c r="B20" s="53"/>
+      <c r="C20" s="54" t="s">
         <v>60</v>
       </c>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="19"/>
+      <c r="D20" s="55"/>
+      <c r="E20" s="55"/>
+      <c r="F20" s="55"/>
+      <c r="G20" s="55"/>
+      <c r="H20" s="56"/>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="6">
@@ -1886,14 +1904,14 @@
       <c r="B21" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="20" t="s">
+      <c r="C21" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="21"/>
+      <c r="D21" s="57"/>
+      <c r="E21" s="57"/>
+      <c r="F21" s="57"/>
+      <c r="G21" s="57"/>
+      <c r="H21" s="58"/>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="6">
@@ -1902,14 +1920,14 @@
       <c r="B22" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="20" t="s">
+      <c r="C22" s="57" t="s">
         <v>61</v>
       </c>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="21"/>
+      <c r="D22" s="57"/>
+      <c r="E22" s="57"/>
+      <c r="F22" s="57"/>
+      <c r="G22" s="57"/>
+      <c r="H22" s="58"/>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="6">
@@ -1918,14 +1936,14 @@
       <c r="B23" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="20" t="s">
+      <c r="C23" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="21"/>
+      <c r="D23" s="57"/>
+      <c r="E23" s="57"/>
+      <c r="F23" s="57"/>
+      <c r="G23" s="57"/>
+      <c r="H23" s="58"/>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="6">
@@ -1934,14 +1952,14 @@
       <c r="B24" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="20" t="s">
+      <c r="C24" s="57" t="s">
         <v>65</v>
       </c>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="21"/>
+      <c r="D24" s="57"/>
+      <c r="E24" s="57"/>
+      <c r="F24" s="57"/>
+      <c r="G24" s="57"/>
+      <c r="H24" s="58"/>
     </row>
     <row r="25" spans="1:8" ht="17.25" customHeight="1" thickBot="1">
       <c r="A25" s="8">
@@ -1950,32 +1968,35 @@
       <c r="B25" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="C25" s="50" t="s">
         <v>65</v>
       </c>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="14"/>
+      <c r="D25" s="50"/>
+      <c r="E25" s="50"/>
+      <c r="F25" s="50"/>
+      <c r="G25" s="50"/>
+      <c r="H25" s="51"/>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:H3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:H4"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="C5:H5"/>
-    <mergeCell ref="C6:H6"/>
-    <mergeCell ref="C7:H7"/>
+    <mergeCell ref="C25:H25"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:H20"/>
+    <mergeCell ref="C21:H21"/>
+    <mergeCell ref="C22:H22"/>
+    <mergeCell ref="C23:H23"/>
+    <mergeCell ref="C24:H24"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="C14:H14"/>
+    <mergeCell ref="C15:H15"/>
+    <mergeCell ref="C16:H16"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="C17:H17"/>
+    <mergeCell ref="C18:H18"/>
+    <mergeCell ref="C19:H19"/>
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="C8:H8"/>
     <mergeCell ref="C9:H9"/>
@@ -1984,6 +2005,419 @@
     <mergeCell ref="C11:H11"/>
     <mergeCell ref="C12:H12"/>
     <mergeCell ref="C13:H13"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="C6:H6"/>
+    <mergeCell ref="C7:H7"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:H3"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:H26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
+  <cols>
+    <col min="1" max="1" width="12.375" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="9" style="4"/>
+    <col min="8" max="8" width="31.25" style="4" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="39" thickBot="1">
+      <c r="A1" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="15"/>
+    </row>
+    <row r="2" spans="1:8" ht="17.25" thickTop="1">
+      <c r="A2" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="17"/>
+      <c r="C2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="19"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" s="20"/>
+    </row>
+    <row r="3" spans="1:8" ht="56.25" customHeight="1" thickBot="1">
+      <c r="A3" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="22"/>
+      <c r="C3" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="25"/>
+    </row>
+    <row r="4" spans="1:8" ht="17.25" thickBot="1">
+      <c r="A4" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="27"/>
+      <c r="C4" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="30"/>
+    </row>
+    <row r="5" spans="1:8" ht="74.25" customHeight="1" thickTop="1">
+      <c r="A5" s="31">
+        <v>42688</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="35"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="32"/>
+      <c r="B6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="36"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="38"/>
+    </row>
+    <row r="7" spans="1:8" ht="17.25" thickBot="1">
+      <c r="A7" s="33"/>
+      <c r="B7" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="39"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="41"/>
+    </row>
+    <row r="8" spans="1:8" ht="24" customHeight="1" thickTop="1">
+      <c r="A8" s="31">
+        <v>42689</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="35"/>
+    </row>
+    <row r="9" spans="1:8" ht="40.5" customHeight="1">
+      <c r="A9" s="32"/>
+      <c r="B9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="38"/>
+    </row>
+    <row r="10" spans="1:8" ht="17.25" thickBot="1">
+      <c r="A10" s="33"/>
+      <c r="B10" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="39"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="41"/>
+    </row>
+    <row r="11" spans="1:8" ht="54" customHeight="1" thickTop="1">
+      <c r="A11" s="31">
+        <v>42690</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="35"/>
+    </row>
+    <row r="12" spans="1:8" ht="126" customHeight="1">
+      <c r="A12" s="32"/>
+      <c r="B12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="38"/>
+    </row>
+    <row r="13" spans="1:8" ht="44.25" customHeight="1" thickBot="1">
+      <c r="A13" s="33"/>
+      <c r="B13" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="41"/>
+    </row>
+    <row r="14" spans="1:8" ht="66" customHeight="1" thickTop="1">
+      <c r="A14" s="31">
+        <v>42691</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="35"/>
+    </row>
+    <row r="15" spans="1:8" ht="45.75" customHeight="1">
+      <c r="A15" s="32"/>
+      <c r="B15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="38"/>
+    </row>
+    <row r="16" spans="1:8" ht="27.75" customHeight="1" thickBot="1">
+      <c r="A16" s="33"/>
+      <c r="B16" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="40"/>
+      <c r="H16" s="41"/>
+    </row>
+    <row r="17" spans="1:8" ht="64.5" customHeight="1" thickTop="1">
+      <c r="A17" s="31">
+        <v>42692</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17" s="43"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="43"/>
+      <c r="H17" s="44"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="32"/>
+      <c r="B18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" s="46"/>
+      <c r="E18" s="46"/>
+      <c r="F18" s="46"/>
+      <c r="G18" s="46"/>
+      <c r="H18" s="47"/>
+    </row>
+    <row r="19" spans="1:8" ht="17.25" thickBot="1">
+      <c r="A19" s="32"/>
+      <c r="B19" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="48"/>
+      <c r="D19" s="48"/>
+      <c r="E19" s="48"/>
+      <c r="F19" s="48"/>
+      <c r="G19" s="48"/>
+      <c r="H19" s="49"/>
+    </row>
+    <row r="20" spans="1:8" ht="39.75" customHeight="1">
+      <c r="A20" s="52" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="53"/>
+      <c r="C20" s="54" t="s">
+        <v>60</v>
+      </c>
+      <c r="D20" s="55"/>
+      <c r="E20" s="55"/>
+      <c r="F20" s="55"/>
+      <c r="G20" s="55"/>
+      <c r="H20" s="56"/>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="6">
+        <v>42695</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="57" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21" s="57"/>
+      <c r="E21" s="57"/>
+      <c r="F21" s="57"/>
+      <c r="G21" s="57"/>
+      <c r="H21" s="58"/>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="6">
+        <v>42696</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="57" t="s">
+        <v>61</v>
+      </c>
+      <c r="D22" s="57"/>
+      <c r="E22" s="57"/>
+      <c r="F22" s="57"/>
+      <c r="G22" s="57"/>
+      <c r="H22" s="58"/>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="6">
+        <v>42697</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="57" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" s="57"/>
+      <c r="E23" s="57"/>
+      <c r="F23" s="57"/>
+      <c r="G23" s="57"/>
+      <c r="H23" s="58"/>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="6">
+        <v>42698</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="57" t="s">
+        <v>65</v>
+      </c>
+      <c r="D24" s="57"/>
+      <c r="E24" s="57"/>
+      <c r="F24" s="57"/>
+      <c r="G24" s="57"/>
+      <c r="H24" s="58"/>
+    </row>
+    <row r="25" spans="1:8" ht="17.25" customHeight="1" thickBot="1">
+      <c r="A25" s="8">
+        <v>42699</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="50" t="s">
+        <v>65</v>
+      </c>
+      <c r="D25" s="50"/>
+      <c r="E25" s="50"/>
+      <c r="F25" s="50"/>
+      <c r="G25" s="50"/>
+      <c r="H25" s="51"/>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="35">
+    <mergeCell ref="C25:H25"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:H20"/>
+    <mergeCell ref="C21:H21"/>
+    <mergeCell ref="C22:H22"/>
+    <mergeCell ref="C23:H23"/>
+    <mergeCell ref="C24:H24"/>
     <mergeCell ref="A14:A16"/>
     <mergeCell ref="C14:H14"/>
     <mergeCell ref="C15:H15"/>
@@ -1992,13 +2426,26 @@
     <mergeCell ref="C17:H17"/>
     <mergeCell ref="C18:H18"/>
     <mergeCell ref="C19:H19"/>
-    <mergeCell ref="C25:H25"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:H20"/>
-    <mergeCell ref="C21:H21"/>
-    <mergeCell ref="C22:H22"/>
-    <mergeCell ref="C23:H23"/>
-    <mergeCell ref="C24:H24"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="C8:H8"/>
+    <mergeCell ref="C9:H9"/>
+    <mergeCell ref="C10:H10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="C11:H11"/>
+    <mergeCell ref="C12:H12"/>
+    <mergeCell ref="C13:H13"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="C6:H6"/>
+    <mergeCell ref="C7:H7"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:H3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -2006,7 +2453,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -2026,282 +2473,282 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="39" thickBot="1">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="48"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="15"/>
     </row>
     <row r="2" spans="1:8" ht="17.25" thickTop="1">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="51" t="s">
+      <c r="B2" s="17"/>
+      <c r="C2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="52"/>
-      <c r="E2" s="50"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="17"/>
       <c r="F2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="51" t="s">
+      <c r="G2" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="H2" s="53"/>
+      <c r="H2" s="20"/>
     </row>
     <row r="3" spans="1:8" ht="56.25" customHeight="1" thickBot="1">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="56" t="s">
+      <c r="B3" s="22"/>
+      <c r="C3" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="58"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="25"/>
     </row>
     <row r="4" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="41"/>
-      <c r="C4" s="42" t="s">
+      <c r="B4" s="27"/>
+      <c r="C4" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="44"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="30"/>
     </row>
     <row r="5" spans="1:8" ht="146.25" customHeight="1" thickTop="1">
-      <c r="A5" s="22">
+      <c r="A5" s="31">
         <v>42681</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="26"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="35"/>
     </row>
     <row r="6" spans="1:8" ht="37.5" customHeight="1">
-      <c r="A6" s="23"/>
+      <c r="A6" s="32"/>
       <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="45"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="28"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="38"/>
     </row>
     <row r="7" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A7" s="24"/>
+      <c r="A7" s="33"/>
       <c r="B7" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="29"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="31"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="41"/>
     </row>
     <row r="8" spans="1:8" ht="54" customHeight="1" thickTop="1">
-      <c r="A8" s="22">
+      <c r="A8" s="31">
         <v>42682</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="C8" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="26"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="35"/>
     </row>
     <row r="9" spans="1:8" ht="66.75" customHeight="1">
-      <c r="A9" s="23"/>
+      <c r="A9" s="32"/>
       <c r="B9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="28"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="38"/>
     </row>
     <row r="10" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A10" s="24"/>
+      <c r="A10" s="33"/>
       <c r="B10" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="29"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="31"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="41"/>
     </row>
     <row r="11" spans="1:8" ht="54" customHeight="1" thickTop="1">
-      <c r="A11" s="22">
+      <c r="A11" s="31">
         <v>42683</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="25" t="s">
+      <c r="C11" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="26"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="35"/>
     </row>
     <row r="12" spans="1:8" ht="66.75" customHeight="1">
-      <c r="A12" s="23"/>
+      <c r="A12" s="32"/>
       <c r="B12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="28"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="38"/>
     </row>
     <row r="13" spans="1:8" ht="44.25" customHeight="1" thickBot="1">
-      <c r="A13" s="24"/>
+      <c r="A13" s="33"/>
       <c r="B13" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="29" t="s">
+      <c r="C13" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="30"/>
-      <c r="E13" s="30"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="30"/>
-      <c r="H13" s="31"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="41"/>
     </row>
     <row r="14" spans="1:8" ht="54" customHeight="1" thickTop="1">
-      <c r="A14" s="22">
+      <c r="A14" s="31">
         <v>42684</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="25" t="s">
+      <c r="C14" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="26"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="35"/>
     </row>
     <row r="15" spans="1:8" ht="66.75" customHeight="1">
-      <c r="A15" s="23"/>
+      <c r="A15" s="32"/>
       <c r="B15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="28"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="38"/>
     </row>
     <row r="16" spans="1:8" ht="53.25" customHeight="1" thickBot="1">
-      <c r="A16" s="24"/>
+      <c r="A16" s="33"/>
       <c r="B16" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="29" t="s">
+      <c r="C16" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="31"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="40"/>
+      <c r="H16" s="41"/>
     </row>
     <row r="17" spans="1:8" ht="18" thickTop="1">
-      <c r="A17" s="22">
+      <c r="A17" s="31">
         <v>42685</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="60" t="s">
+      <c r="C17" s="59" t="s">
         <v>50</v>
       </c>
-      <c r="D17" s="60"/>
-      <c r="E17" s="60"/>
-      <c r="F17" s="60"/>
-      <c r="G17" s="60"/>
-      <c r="H17" s="61"/>
+      <c r="D17" s="59"/>
+      <c r="E17" s="59"/>
+      <c r="F17" s="59"/>
+      <c r="G17" s="59"/>
+      <c r="H17" s="60"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="23"/>
+      <c r="A18" s="32"/>
       <c r="B18" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="35"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="37"/>
+      <c r="C18" s="45"/>
+      <c r="D18" s="46"/>
+      <c r="E18" s="46"/>
+      <c r="F18" s="46"/>
+      <c r="G18" s="46"/>
+      <c r="H18" s="47"/>
     </row>
     <row r="19" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A19" s="24"/>
+      <c r="A19" s="33"/>
       <c r="B19" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="27"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="27"/>
-      <c r="H19" s="28"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="37"/>
+      <c r="H19" s="38"/>
     </row>
     <row r="20" spans="1:8" ht="39.75" customHeight="1" thickTop="1">
-      <c r="A20" s="15" t="s">
+      <c r="A20" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="16"/>
-      <c r="C20" s="17" t="s">
+      <c r="B20" s="53"/>
+      <c r="C20" s="54" t="s">
         <v>67</v>
       </c>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="19"/>
+      <c r="D20" s="55"/>
+      <c r="E20" s="55"/>
+      <c r="F20" s="55"/>
+      <c r="G20" s="55"/>
+      <c r="H20" s="56"/>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="6">
@@ -2310,14 +2757,14 @@
       <c r="B21" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="20" t="s">
+      <c r="C21" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="21"/>
+      <c r="D21" s="57"/>
+      <c r="E21" s="57"/>
+      <c r="F21" s="57"/>
+      <c r="G21" s="57"/>
+      <c r="H21" s="58"/>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="6">
@@ -2326,14 +2773,14 @@
       <c r="B22" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="20" t="s">
+      <c r="C22" s="57" t="s">
         <v>42</v>
       </c>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="21"/>
+      <c r="D22" s="57"/>
+      <c r="E22" s="57"/>
+      <c r="F22" s="57"/>
+      <c r="G22" s="57"/>
+      <c r="H22" s="58"/>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="6">
@@ -2342,14 +2789,14 @@
       <c r="B23" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="20" t="s">
+      <c r="C23" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="21"/>
+      <c r="D23" s="57"/>
+      <c r="E23" s="57"/>
+      <c r="F23" s="57"/>
+      <c r="G23" s="57"/>
+      <c r="H23" s="58"/>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="6">
@@ -2358,14 +2805,14 @@
       <c r="B24" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="20" t="s">
+      <c r="C24" s="57" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="21"/>
+      <c r="D24" s="57"/>
+      <c r="E24" s="57"/>
+      <c r="F24" s="57"/>
+      <c r="G24" s="57"/>
+      <c r="H24" s="58"/>
     </row>
     <row r="25" spans="1:8" ht="17.25" customHeight="1" thickBot="1">
       <c r="A25" s="6">
@@ -2374,32 +2821,35 @@
       <c r="B25" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="59" t="s">
+      <c r="C25" s="61" t="s">
         <v>45</v>
       </c>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="14"/>
+      <c r="D25" s="50"/>
+      <c r="E25" s="50"/>
+      <c r="F25" s="50"/>
+      <c r="G25" s="50"/>
+      <c r="H25" s="51"/>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:H3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:H4"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="C5:H5"/>
-    <mergeCell ref="C6:H6"/>
-    <mergeCell ref="C7:H7"/>
+    <mergeCell ref="C25:H25"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:H20"/>
+    <mergeCell ref="C21:H21"/>
+    <mergeCell ref="C22:H22"/>
+    <mergeCell ref="C23:H23"/>
+    <mergeCell ref="C24:H24"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="C14:H14"/>
+    <mergeCell ref="C15:H15"/>
+    <mergeCell ref="C16:H16"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="C17:H17"/>
+    <mergeCell ref="C18:H18"/>
+    <mergeCell ref="C19:H19"/>
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="C8:H8"/>
     <mergeCell ref="C9:H9"/>
@@ -2408,21 +2858,18 @@
     <mergeCell ref="C11:H11"/>
     <mergeCell ref="C12:H12"/>
     <mergeCell ref="C13:H13"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="C14:H14"/>
-    <mergeCell ref="C15:H15"/>
-    <mergeCell ref="C16:H16"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="C17:H17"/>
-    <mergeCell ref="C18:H18"/>
-    <mergeCell ref="C19:H19"/>
-    <mergeCell ref="C25:H25"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:H20"/>
-    <mergeCell ref="C21:H21"/>
-    <mergeCell ref="C22:H22"/>
-    <mergeCell ref="C23:H23"/>
-    <mergeCell ref="C24:H24"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="C6:H6"/>
+    <mergeCell ref="C7:H7"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:H3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -2430,7 +2877,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -2450,106 +2897,106 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="39" thickBot="1">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="48"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="15"/>
     </row>
     <row r="2" spans="1:8" ht="17.25" thickTop="1">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="51" t="s">
+      <c r="B2" s="17"/>
+      <c r="C2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="52"/>
-      <c r="E2" s="50"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="17"/>
       <c r="F2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="51" t="s">
+      <c r="G2" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="53"/>
+      <c r="H2" s="20"/>
     </row>
     <row r="3" spans="1:8" ht="56.25" customHeight="1" thickBot="1">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="56" t="s">
+      <c r="B3" s="22"/>
+      <c r="C3" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="58"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="25"/>
     </row>
     <row r="4" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="41"/>
-      <c r="C4" s="42" t="s">
+      <c r="B4" s="27"/>
+      <c r="C4" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="44"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="30"/>
     </row>
     <row r="5" spans="1:8" ht="45" customHeight="1" thickTop="1">
-      <c r="A5" s="22">
+      <c r="A5" s="31">
         <v>42674</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="26"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="35"/>
     </row>
     <row r="6" spans="1:8" ht="37.5" customHeight="1">
-      <c r="A6" s="23"/>
+      <c r="A6" s="32"/>
       <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="45" t="s">
+      <c r="C6" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="28"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="38"/>
     </row>
     <row r="7" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A7" s="24"/>
+      <c r="A7" s="33"/>
       <c r="B7" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="31"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="41"/>
     </row>
     <row r="8" spans="1:8" ht="54" customHeight="1" thickTop="1">
       <c r="A8" s="62">
@@ -2558,42 +3005,42 @@
       <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="C8" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="26"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="35"/>
     </row>
     <row r="9" spans="1:8" ht="66.75" customHeight="1">
       <c r="A9" s="63"/>
       <c r="B9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="28"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="38"/>
     </row>
     <row r="10" spans="1:8" ht="17.25" thickBot="1">
       <c r="A10" s="64"/>
       <c r="B10" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="29" t="s">
+      <c r="C10" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="31"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="41"/>
     </row>
     <row r="11" spans="1:8" ht="54" customHeight="1" thickTop="1">
       <c r="A11" s="62">
@@ -2602,42 +3049,42 @@
       <c r="B11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="25" t="s">
+      <c r="C11" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="26"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="35"/>
     </row>
     <row r="12" spans="1:8" ht="66.75" customHeight="1">
       <c r="A12" s="63"/>
       <c r="B12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="27" t="s">
+      <c r="C12" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="28"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="38"/>
     </row>
     <row r="13" spans="1:8" ht="17.25" thickBot="1">
       <c r="A13" s="64"/>
       <c r="B13" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="29" t="s">
+      <c r="C13" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="30"/>
-      <c r="E13" s="30"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="30"/>
-      <c r="H13" s="31"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="41"/>
     </row>
     <row r="14" spans="1:8" ht="54" customHeight="1" thickTop="1">
       <c r="A14" s="62">
@@ -2646,98 +3093,98 @@
       <c r="B14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="25" t="s">
+      <c r="C14" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="26"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="35"/>
     </row>
     <row r="15" spans="1:8" ht="66.75" customHeight="1">
       <c r="A15" s="63"/>
       <c r="B15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="27" t="s">
+      <c r="C15" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="27"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="28"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="38"/>
     </row>
     <row r="16" spans="1:8" ht="17.25" thickBot="1">
       <c r="A16" s="64"/>
       <c r="B16" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="29" t="s">
+      <c r="C16" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="31"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="40"/>
+      <c r="H16" s="41"/>
     </row>
     <row r="17" spans="1:8" ht="18" thickTop="1">
-      <c r="A17" s="23">
+      <c r="A17" s="32">
         <v>42678</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="60" t="s">
+      <c r="C17" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="60"/>
-      <c r="E17" s="60"/>
-      <c r="F17" s="60"/>
-      <c r="G17" s="60"/>
-      <c r="H17" s="61"/>
+      <c r="D17" s="59"/>
+      <c r="E17" s="59"/>
+      <c r="F17" s="59"/>
+      <c r="G17" s="59"/>
+      <c r="H17" s="60"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="23"/>
+      <c r="A18" s="32"/>
       <c r="B18" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="35"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="37"/>
+      <c r="C18" s="45"/>
+      <c r="D18" s="46"/>
+      <c r="E18" s="46"/>
+      <c r="F18" s="46"/>
+      <c r="G18" s="46"/>
+      <c r="H18" s="47"/>
     </row>
     <row r="19" spans="1:8" ht="17.25" thickBot="1">
       <c r="A19" s="65"/>
       <c r="B19" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="27" t="s">
+      <c r="C19" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="D19" s="27"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="27"/>
-      <c r="H19" s="28"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="37"/>
+      <c r="H19" s="38"/>
     </row>
     <row r="20" spans="1:8" ht="32.25" customHeight="1">
-      <c r="A20" s="15" t="s">
+      <c r="A20" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="16"/>
-      <c r="C20" s="17" t="s">
+      <c r="B20" s="53"/>
+      <c r="C20" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="19"/>
+      <c r="D20" s="55"/>
+      <c r="E20" s="55"/>
+      <c r="F20" s="55"/>
+      <c r="G20" s="55"/>
+      <c r="H20" s="56"/>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="6">
@@ -2746,14 +3193,14 @@
       <c r="B21" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="20" t="s">
+      <c r="C21" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="21"/>
+      <c r="D21" s="57"/>
+      <c r="E21" s="57"/>
+      <c r="F21" s="57"/>
+      <c r="G21" s="57"/>
+      <c r="H21" s="58"/>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="6">
@@ -2762,14 +3209,14 @@
       <c r="B22" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="20" t="s">
+      <c r="C22" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="21"/>
+      <c r="D22" s="57"/>
+      <c r="E22" s="57"/>
+      <c r="F22" s="57"/>
+      <c r="G22" s="57"/>
+      <c r="H22" s="58"/>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="6">
@@ -2778,14 +3225,14 @@
       <c r="B23" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="20" t="s">
+      <c r="C23" s="57" t="s">
         <v>32</v>
       </c>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="21"/>
+      <c r="D23" s="57"/>
+      <c r="E23" s="57"/>
+      <c r="F23" s="57"/>
+      <c r="G23" s="57"/>
+      <c r="H23" s="58"/>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="6">
@@ -2794,14 +3241,14 @@
       <c r="B24" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="20" t="s">
+      <c r="C24" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="21"/>
+      <c r="D24" s="57"/>
+      <c r="E24" s="57"/>
+      <c r="F24" s="57"/>
+      <c r="G24" s="57"/>
+      <c r="H24" s="58"/>
     </row>
     <row r="25" spans="1:8" ht="17.25" customHeight="1" thickBot="1">
       <c r="A25" s="8">
@@ -2810,33 +3257,26 @@
       <c r="B25" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="59" t="s">
+      <c r="C25" s="61" t="s">
         <v>35</v>
       </c>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="14"/>
+      <c r="D25" s="50"/>
+      <c r="E25" s="50"/>
+      <c r="F25" s="50"/>
+      <c r="G25" s="50"/>
+      <c r="H25" s="51"/>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="C21:H21"/>
-    <mergeCell ref="C22:H22"/>
-    <mergeCell ref="C23:H23"/>
-    <mergeCell ref="C24:H24"/>
-    <mergeCell ref="C25:H25"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C3:H3"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="C4:H4"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C9:H9"/>
+    <mergeCell ref="C12:H12"/>
+    <mergeCell ref="C15:H15"/>
+    <mergeCell ref="C20:H20"/>
+    <mergeCell ref="C19:H19"/>
+    <mergeCell ref="C18:H18"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="A5:A7"/>
@@ -2853,12 +3293,19 @@
     <mergeCell ref="C16:H16"/>
     <mergeCell ref="C17:H17"/>
     <mergeCell ref="C6:H6"/>
-    <mergeCell ref="C9:H9"/>
-    <mergeCell ref="C12:H12"/>
-    <mergeCell ref="C15:H15"/>
-    <mergeCell ref="C20:H20"/>
-    <mergeCell ref="C19:H19"/>
-    <mergeCell ref="C18:H18"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C21:H21"/>
+    <mergeCell ref="C22:H22"/>
+    <mergeCell ref="C23:H23"/>
+    <mergeCell ref="C24:H24"/>
+    <mergeCell ref="C25:H25"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[map] mem rick fix
</commit_message>
<xml_diff>
--- a/doc/_meeting_weekly_doc/N2Team_WeeklySchedule_YSR.xlsx
+++ b/doc/_meeting_weekly_doc/N2Team_WeeklySchedule_YSR.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="-15" windowWidth="28020" windowHeight="3765"/>
+    <workbookView xWindow="60" yWindow="-15" windowWidth="28020" windowHeight="3765" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="일정" sheetId="6" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="279">
   <si>
     <t xml:space="preserve">작성자 </t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1331,6 +1331,15 @@
   </si>
   <si>
     <t>수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* HeightMap 이해</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* HeightMap 이해 &amp; 코딩 
+* 오브젝트 배치 &amp; Frustum culling</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3135,11 +3144,11 @@
   </sheetPr>
   <dimension ref="A1:BC128"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="O3" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="M3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="O6" sqref="N6:O6"/>
+      <selection pane="bottomRight" activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -10001,9 +10010,9 @@
   </sheetPr>
   <dimension ref="A1:L56"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A23" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H43" sqref="H43"/>
+      <selection pane="topRight" activeCell="E41" sqref="E41:E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="41" defaultRowHeight="16.5"/>
@@ -10896,8 +10905,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13:H13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9:H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -10973,7 +10982,9 @@
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="68"/>
+      <c r="C5" s="68" t="s">
+        <v>277</v>
+      </c>
       <c r="D5" s="68"/>
       <c r="E5" s="68"/>
       <c r="F5" s="68"/>
@@ -11011,7 +11022,9 @@
       <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="68"/>
+      <c r="C8" s="68" t="s">
+        <v>278</v>
+      </c>
       <c r="D8" s="68"/>
       <c r="E8" s="68"/>
       <c r="F8" s="68"/>

</xml_diff>